<commit_message>
added trend epi report in xlsx and sas format
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
   <si>
     <t>dir</t>
   </si>
@@ -237,6 +237,24 @@
   </si>
   <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUT/CountSummary</t>
+  </si>
+  <si>
+    <t>basic_CRF_extract.xlsx</t>
+  </si>
+  <si>
+    <t>trend_epi</t>
+  </si>
+  <si>
+    <t>keep_only_trend_epi_cols</t>
+  </si>
+  <si>
+    <t>basic_CRF_extract.sas7bdat</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/EPI SUMMARY/Trend analysis/_Current/_Source Data/CaseReportForm</t>
+  </si>
+  <si>
+    <t>save_sas7bdat</t>
   </si>
 </sst>
 </file>
@@ -554,17 +572,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1136,13 +1154,25 @@
       <c r="F16" t="s">
         <v>49</v>
       </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
       <c r="I16" t="s">
         <v>66</v>
       </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
       <c r="K16" t="s">
         <v>66</v>
       </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
       <c r="M16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1168,6 +1198,9 @@
       <c r="H17" t="s">
         <v>66</v>
       </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
       <c r="J17" t="s">
         <v>66</v>
       </c>
@@ -1177,7 +1210,95 @@
       <c r="L17" t="s">
         <v>66</v>
       </c>
+      <c r="M17" t="s">
+        <v>66</v>
+      </c>
       <c r="N17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor corrections to code (path and missing ')
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Documents\Projects\covid_cases_data_extracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAUJLA\Documents\HPOC Data Science\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="73">
   <si>
     <t>dir</t>
   </si>
@@ -209,9 +209,6 @@
     <t>format(Sys.Date() ,'%d%B%Y')</t>
   </si>
   <si>
-    <t>format(Sys.Date() ,'%Y-%m-%d)</t>
-  </si>
-  <si>
     <t>Sun</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUT/CountSummary</t>
-  </si>
-  <si>
     <t>basic_CRF_extract.xlsx</t>
   </si>
   <si>
@@ -255,6 +249,9 @@
   </si>
   <si>
     <t>save_sas7bdat</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/CountSummary</t>
   </si>
 </sst>
 </file>
@@ -574,28 +571,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -618,28 +615,28 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>64</v>
       </c>
-      <c r="N1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -656,28 +653,28 @@
         <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -697,28 +694,28 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -735,28 +732,28 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -776,28 +773,28 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -814,28 +811,28 @@
         <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -855,28 +852,28 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -896,28 +893,28 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -937,28 +934,28 @@
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -975,28 +972,28 @@
         <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1013,28 +1010,28 @@
         <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1051,10 +1048,10 @@
         <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1071,10 +1068,10 @@
         <v>39</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1091,10 +1088,10 @@
         <v>39</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1114,28 +1111,28 @@
         <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1146,37 +1143,37 @@
         <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
         <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1196,110 +1193,110 @@
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
         <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>72</v>
       </c>
       <c r="E18" t="s">
         <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
         <v>70</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>48</v>
       </c>
       <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="G19" t="s">
-        <v>73</v>
-      </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added imputation to datahub extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="75">
   <si>
     <t>dir</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>save_sas7bdat</t>
+  </si>
+  <si>
+    <t>make_data_hub</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M11" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1102,10 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
fix excel file issues #2
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAUJLA\Documents\HPOC Data Science\covid_cases_data_extracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Documents\Projects\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="74">
   <si>
     <t>dir</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/CountSummary</t>
+  </si>
+  <si>
+    <t>make_data_hub</t>
   </si>
 </sst>
 </file>
@@ -571,28 +574,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -636,7 +639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -674,7 +677,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -715,7 +718,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -753,7 +756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -794,7 +797,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -832,7 +835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -873,7 +876,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -914,7 +917,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -955,7 +958,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -993,7 +996,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1091,12 +1094,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>
@@ -1132,7 +1138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1173,7 +1179,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1255,7 +1261,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Trend epi - changed to only mon and tues; Web epi - added function to select certain columns
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Documents\Projects\covid_cases_data_extracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAUJLA\Documents\HPOC Data Science\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
   <si>
     <t>dir</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>make_data_hub</t>
+  </si>
+  <si>
+    <t>keep_only_web_epi_cols</t>
   </si>
 </sst>
 </file>
@@ -574,28 +577,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -639,13 +642,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
@@ -677,13 +683,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
@@ -718,7 +727,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -756,7 +765,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -797,7 +806,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -835,7 +844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -876,7 +885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -917,7 +926,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -958,7 +967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1239,29 +1248,14 @@
       <c r="F18" t="s">
         <v>66</v>
       </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
       <c r="I18" t="s">
         <v>65</v>
       </c>
-      <c r="J18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" t="s">
-        <v>65</v>
-      </c>
       <c r="L18" t="s">
         <v>65</v>
       </c>
-      <c r="M18" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1283,25 +1277,10 @@
       <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="H19" t="s">
-        <v>65</v>
-      </c>
       <c r="I19" t="s">
         <v>65</v>
       </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
-      </c>
       <c r="L19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed trend epi sas extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="73">
   <si>
     <t>dir</t>
   </si>
@@ -242,13 +242,7 @@
     <t>keep_only_trend_epi_cols</t>
   </si>
   <si>
-    <t>basic_CRF_extract.sas7bdat</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/EPI SUMMARY/Trend analysis/_Current/_Source Data/CaseReportForm</t>
-  </si>
-  <si>
-    <t>save_sas7bdat</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/CountSummary</t>
@@ -575,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,7 +644,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -691,7 +685,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -738,7 +732,7 @@
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
@@ -755,30 +749,39 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>71</v>
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
       </c>
       <c r="I5" t="s">
         <v>65</v>
       </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
       <c r="L5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -796,7 +799,10 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
       <c r="H6" t="s">
         <v>65</v>
@@ -822,22 +828,19 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
         <v>65</v>
@@ -875,7 +878,10 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
       </c>
       <c r="H8" t="s">
         <v>65</v>
@@ -901,22 +907,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
         <v>65</v>
@@ -951,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -983,22 +989,19 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
         <v>65</v>
@@ -1030,7 +1033,7 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1062,59 +1065,41 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1126,7 +1111,7 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>57</v>
@@ -1140,45 +1125,66 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
       </c>
       <c r="L16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" t="s">
+        <v>65</v>
+      </c>
+      <c r="N16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H17" t="s">
         <v>65</v>
@@ -1204,22 +1210,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
         <v>65</v>
@@ -1240,47 +1246,6 @@
         <v>65</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix out of range dates in imputed date columns
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAUJLA\Documents\HPOC Data Science\covid_cases_data_extracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Projects\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="73">
   <si>
     <t>dir</t>
   </si>
@@ -572,27 +572,27 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E5" sqref="A5:XFD5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -636,7 +636,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -677,7 +677,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -721,7 +721,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -743,11 +743,8 @@
       <c r="I4" t="s">
         <v>65</v>
       </c>
-      <c r="L4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -785,7 +782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -826,7 +823,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -864,7 +861,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -905,7 +902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -946,7 +943,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -987,7 +984,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1063,7 +1060,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1083,7 +1080,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1167,7 +1164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1208,7 +1205,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
web epi schedule changed to only friday extracts
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hswerdfe\Projects\covid_cases_data_extracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAUJLA\Documents\HPOC Data Science\covid_cases_data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
   <si>
     <t>dir</t>
   </si>
@@ -572,27 +572,27 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="217.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -636,7 +636,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -655,29 +655,11 @@
       <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
       <c r="M2" t="s">
         <v>65</v>
       </c>
-      <c r="N2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -699,29 +681,11 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
-        <v>65</v>
-      </c>
       <c r="M3" t="s">
         <v>65</v>
       </c>
-      <c r="N3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -743,8 +707,11 @@
       <c r="I4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -782,7 +749,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -823,7 +790,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -861,7 +828,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -902,7 +869,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -943,7 +910,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -984,7 +951,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1060,7 +1027,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1080,7 +1047,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1100,7 +1067,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1120,7 +1087,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1164,7 +1131,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1205,7 +1172,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
statcan table select only classification='confirmed' cases
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -128,9 +128,6 @@
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/STATCAN</t>
   </si>
   <si>
-    <t>select * from statscan;</t>
-  </si>
-  <si>
     <t>WHO</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>qry_allcases {suffix}_DISCOVER.rds</t>
   </si>
   <si>
-    <t>Weekly Extended Dataset_{suffix}_DISOCVER.xlsx</t>
-  </si>
-  <si>
     <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
@@ -252,6 +246,12 @@
   </si>
   <si>
     <t>keep_only_web_epi_cols</t>
+  </si>
+  <si>
+    <t>select * from statscan where classification='confirmed';</t>
+  </si>
+  <si>
+    <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,25 +615,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -644,19 +644,19 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -667,48 +667,48 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -728,25 +728,25 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -769,25 +769,25 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -804,28 +804,28 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -842,31 +842,31 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -883,31 +883,31 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -924,31 +924,31 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -965,28 +965,28 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1003,28 +1003,28 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1032,185 +1032,185 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
-      </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed path of db_errs output
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -188,9 +188,6 @@
     <t>db_errs</t>
   </si>
   <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/MS ACCESS/OUTPUT/db_errs</t>
-  </si>
-  <si>
     <t>db_errs {suffix}.xlsx</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/DISCOVER/Data Quality/db_errs</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,25 +615,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -644,7 +644,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -656,7 +656,7 @@
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -667,7 +667,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -682,33 +682,33 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
         <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -728,25 +728,25 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -769,25 +769,25 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -807,25 +807,25 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -848,25 +848,25 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -883,31 +883,31 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -924,31 +924,31 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -968,25 +968,25 @@
         <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1006,25 +1006,25 @@
         <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1032,19 +1032,19 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1058,13 +1058,13 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
         <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1078,13 +1078,13 @@
         <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
         <v>37</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -1095,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -1110,25 +1110,25 @@
         <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1142,7 +1142,7 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
@@ -1151,25 +1151,25 @@
         <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1180,37 +1180,37 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file name typo correction
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -149,9 +149,6 @@
     <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
-    <t>{suffix}_HCDaily_DICOVER.xlsx</t>
-  </si>
-  <si>
     <t>Domestic surveillance data - {suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/DISCOVER/Data Quality/db_errs</t>
+  </si>
+  <si>
+    <t>{suffix}_HCDaily_DISCOVER.xlsx</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,25 +615,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>60</v>
-      </c>
-      <c r="N1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -644,19 +644,19 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -667,48 +667,48 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -728,25 +728,25 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -769,25 +769,25 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -807,25 +807,25 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -848,25 +848,25 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -883,31 +883,31 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -924,31 +924,31 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -965,28 +965,28 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1003,28 +1003,28 @@
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1032,19 +1032,19 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1058,13 +1058,13 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
         <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1078,139 +1078,139 @@
         <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
         <v>37</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
         <v>43</v>
       </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" t="s">
-        <v>45</v>
-      </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added trend epi and modelling extracts
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="75">
   <si>
     <t>dir</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>{suffix}_HCDaily_DISCOVER.xlsx</t>
+  </si>
+  <si>
+    <t>basic_CRF_extract.rds</t>
+  </si>
+  <si>
+    <t>https://storphacidpcbns02.blob.core.windows.net/hcdaily</t>
   </si>
 </sst>
 </file>
@@ -569,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,39 +719,30 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
       <c r="I5" t="s">
         <v>61</v>
       </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
       <c r="L5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -763,10 +760,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
         <v>61</v>
@@ -792,19 +786,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
       </c>
       <c r="H7" t="s">
         <v>61</v>
@@ -842,10 +839,7 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
         <v>61</v>
@@ -871,22 +865,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
       </c>
       <c r="H9" t="s">
         <v>61</v>
@@ -921,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>52</v>
@@ -953,19 +947,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
         <v>61</v>
@@ -991,59 +988,41 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" t="s">
-        <v>61</v>
-      </c>
-      <c r="M12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1055,7 +1034,7 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
@@ -1069,45 +1048,57 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" t="s">
+        <v>61</v>
       </c>
       <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
@@ -1133,22 +1124,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>44</v>
       </c>
       <c r="H17" t="s">
         <v>61</v>
@@ -1174,47 +1165,135 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>21</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>50</v>
       </c>
-      <c r="H18" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" t="s">
-        <v>61</v>
-      </c>
-      <c r="M18" t="s">
-        <v>61</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modelling saved to azure
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
   <si>
     <t>dir</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>https://storphacidpcbns02.blob.core.windows.net/hcdaily</t>
+  </si>
+  <si>
+    <t>save_azure_modelling</t>
   </si>
 </sst>
 </file>
@@ -577,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1142,7 @@
         <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
remove blank space in modelling extract name, as requested
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="77">
   <si>
     <t>dir</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>save_azure_modelling</t>
+  </si>
+  <si>
+    <t>DomesticSurveillanceData_{suffix}_DISCOVER.xlsx</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1142,7 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
save compressed csv for azure modelling extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -263,7 +263,7 @@
     <t>save_azure_modelling</t>
   </si>
   <si>
-    <t>DomesticSurveillanceData_{suffix}_DISCOVER.xlsx</t>
+    <t>DomesticSurveillanceData_{suffix}_DISCOVER_test.csv.bz2</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
trend epi daily rds schedule updated
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="77">
   <si>
     <t>dir</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,10 +745,25 @@
       <c r="G5" t="s">
         <v>10</v>
       </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
       <c r="I5" t="s">
         <v>61</v>
       </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
       <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trend epi extract rename
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -221,9 +221,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>basic_CRF_extract.xlsx</t>
-  </si>
-  <si>
     <t>trend_epi</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>{suffix}_HCDaily_DISCOVER.xlsx</t>
   </si>
   <si>
-    <t>basic_CRF_extract.rds</t>
-  </si>
-  <si>
     <t>https://storphacidpcbns02.blob.core.windows.net/hcdaily</t>
   </si>
   <si>
@@ -264,6 +258,12 @@
   </si>
   <si>
     <t>DomesticSurveillanceData_{suffix}_DISCOVER_test.csv.bz2</t>
+  </si>
+  <si>
+    <t>trend_extract.rds</t>
+  </si>
+  <si>
+    <t>trend_extract.xlsx</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -679,7 +679,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -699,22 +699,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
         <v>61</v>
@@ -725,22 +725,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -942,7 +942,7 @@
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
         <v>61</v>
@@ -983,7 +983,7 @@
         <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
         <v>61</v>
@@ -1012,7 +1012,7 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -1021,7 +1021,7 @@
         <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
         <v>61</v>
@@ -1151,16 +1151,16 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
         <v>61</v>
@@ -1192,7 +1192,7 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
@@ -1239,7 +1239,7 @@
         <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -1280,7 +1280,7 @@
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
SQL updates - exclude PEI variables
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -71,18 +71,12 @@
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE</t>
   </si>
   <si>
-    <t>select * from all_cases_web;</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/SAS_Analysis/Domestic data</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DASHBOARD</t>
   </si>
   <si>
-    <t>select * from all_cases;</t>
-  </si>
-  <si>
     <t>nm</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>Dashboard</t>
   </si>
   <si>
-    <t>select * from data_hub;</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/Data Requests/SituationalAwareness Dashboard Daily Extract</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t>L:/HPOC/Active Events/001-20 COVID-19/Dashboard</t>
   </si>
   <si>
-    <t>select * from modelling_data;</t>
-  </si>
-  <si>
     <t>STATCAN</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/WHO</t>
   </si>
   <si>
-    <t>select * from who;</t>
-  </si>
-  <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
   </si>
   <si>
@@ -239,9 +224,6 @@
     <t>keep_only_web_epi_cols</t>
   </si>
   <si>
-    <t>select * from statscan where classification='confirmed';</t>
-  </si>
-  <si>
     <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
@@ -264,6 +246,481 @@
   </si>
   <si>
     <t>trend_extract.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT phacid,
+pt,
+episodedate,
+classification,
+sex2,
+agegroup10,
+age,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupation2 END) AS occupation2,
+healthcare_worker2,
+ltc_resident2,
+asymptomatic2,
+onsetdate2,
+symcough,
+symfever,
+symchills,
+symsorethroat,
+symrunnynose,
+symshortnessofbreath,
+symnausea,
+symheadache,
+symweakness,
+sympain,
+symirritability,
+symdiarrhea,
+symother,
+symotherspec,
+hospstatus,
+disposition2,
+recoverydate2,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat2 END) AS exposure_cat2
+FROM statscan WHERE  classification='confirmed';</t>
+  </si>
+  <si>
+    <t>SELECT phacid,
+episodedate,
+episodetype,
+sex_excunk,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
+symcough,
+symfever,
+symchills,
+symsorethroat,
+symrunnynose,
+symshortnessofbreath,
+symnausea,
+symheadache,
+symweakness,
+sympain,
+symirritability,
+symdiarrhea,
+symother,
+symotherspec,
+agegroup10,
+agegroup20,
+mechanicalvent,
+hospstatus,
+coviddeath,
+disposition,
+pt,
+last_refreshed
+FROM all_cases_web;</t>
+  </si>
+  <si>
+    <t>SELECT phacid,
+pt,
+ptcaseid,
+phacreporteddate,
+phacreporteddate_epiweek,
+cluster,
+outbreakid,
+outbreak_associated,
+healthregion,
+reporteddate,
+testingreason,
+testingreasonspec,
+classification,
+residency,
+residencecountry,
+detectedatentry,
+dateofentry,
+pointofentrylocation,
+sex,
+gender,
+sexgender,
+age,
+ageunit,
+agegrouping,
+agegroup10,
+agegroup20,
+age_years,
+indigenous,
+(CASE WHEN pt = 'pe' THEN NULL ELSE indigenousidentity END) AS indigenousidentity,
+(CASE WHEN pt = 'pe' THEN NULL ELSE residence_reservecommunitycrownland END) AS residence_reservecommunitycrownland,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupation END) AS occupation,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupationspec END) AS occupationspec,
+occupationhcw,
+occupationhcwrole,
+ltc_resident,
+(CASE WHEN pt = 'pe' THEN NULL ELSE race END) AS race,
+dwellingtype,
+(CASE WHEN pt = 'pe' THEN NULL ELSE fsa END) AS fsa,
+onsetdate,
+onsetdate_epiweek,
+episodedate,
+episodedate_epiweek,
+episodetype,
+earliestdate,
+hosp,
+hospstartdate,
+hospenddate,
+hospstatus,
+hospitalized,
+intensivecareunit,
+icu,
+icustartdate,
+icuenddate,
+isolation,
+isolationstartdate,
+isolationenddate,
+mechanicalvent,
+ventstartdate,
+ventenddate,
+coviddeath,
+disposition,
+recoverydate,
+deathresp,
+deathcause,
+deathdate,
+death,
+travel,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposurecountry END) AS exposurecountry,
+(CASE WHEN pt = 'pe' THEN NULL ELSE location END) AS location,
+travel_domestic,
+travel_international,
+closecontactcase,
+closecontacttravel,
+animalcontact,
+(CASE WHEN pt = 'pe' THEN NULL ELSE known_contact END) AS known_contact,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
+exposure_linked,
+numberofcontacts,
+healthfacilityexposure,
+earliestlabtestresultdate,
+labtestresultdate_epiweek,
+earliestlabcollectiondate,
+labspecimencollectiondate_epiweek,
+minlabname,
+minassay,
+labspecimentype1,
+labtestmethod1,
+labtestresult1,
+rfcardiacdisease,
+rfneurodisorder,
+rfdiabetes,
+rfimmunodef,
+rfliverdisease,
+rfmalignancy,
+rfpostpartum,
+rfpregnancy,
+rfpregtrimester,
+rfrenaldisease,
+rfrespdisease,
+rfvaping,
+rfasthma,
+rfcardiovasculardisease,
+rfcerebrovasculardisease,
+rfchronickidneydisease,
+rfcopd,
+rfhypertension,
+rfobesity,
+rfproblematicsubstanceuse,
+rfsicklecelldisease,
+rfsmokingtobacco,
+rfother,
+rfotherspec,
+rfcount,
+comp_riskfactors,
+asymptomatic2,
+asymptomatic,
+symcount,
+symcough,
+symfever,
+symchills,
+symsorethroat,
+symrunnynose,
+symshortnessofbreath,
+symnausea,
+symheadache,
+symweakness,
+sympain,
+symirritability,
+symdiarrhea,
+symconfusion,
+symchestpain,
+symdizziness,
+symageusia,
+symanosmia,
+symmusclepain,
+symbodyaches,
+symjointpain,
+syminappetence,
+symfatigue,
+symsweats,
+symlocalizedpain,
+symear,
+symnosebleed,
+symeye,
+symcongestion,
+symmalaise,
+symanorexia,
+symskinreactions,
+symsneezing,
+symbreathing,
+symother,
+symotherspec,
+dxlungausc,
+dxlungauscspec,
+dxmentalstatus,
+dxmentalstatusspec,
+dxpneumonia,
+dxpneumoniaspec,
+dxcoma,
+dxcomaspec,
+dxconjunctinjection,
+dxconjunctinjectionspec,
+dxards,
+dxardsspec,
+dxdyspnea,
+dxdyspneaspec,
+dxencephalitis,
+dxencephalitisspec,
+dxhypotension,
+dxhypotensionspec,
+dxpharyngeal,
+dxpharyngealspec,
+dxrenalfailure,
+dxrenalfailurespec,
+dxseizure,
+dxseizurespec,
+dxsepsis,
+dxsepsisspec,
+dxtachypnea,
+dxtachypneaspec,
+dxother,
+dxotherspec,
+contactsetting,
+minsettingspec,
+mincontactcaseid,
+earliestfirstcontactdate,
+latestcontactdate,
+last_refreshed
+FROM all_cases;</t>
+  </si>
+  <si>
+    <t>SELECT episodedate,
+classification,
+pt,
+sexgender2,
+agegroup10,
+age,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupation2 END) AS occupation2,
+occupationhcw,
+ltc_resident,
+asymptomatic2,
+onsetdate2,
+asymptomatic,
+symcough,
+symfever,
+symchills,
+symsorethroat,
+symrunnynose,
+symshortnessofbreath,
+symnausea,
+symheadache,
+symweakness,
+sympain,
+symirritability,
+symdiarrhea,
+symother,
+symotherspec,
+hospstatus,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat2 END) AS exposure_cat2,
+disposition2,
+recoverydate2
+FROM data_hub;</t>
+  </si>
+  <si>
+    <t>SELECT report_date,
+report_orginst,
+report_test_reason,
+report_test_reason_other,
+report_country,
+report_diag_class,
+report_pointofentry,
+report_pointofentry_date,
+patinfo_id,
+patinfo_dob,
+patinfo_ageonset,
+patinfo_ageonsetunit,
+patinfo_sex,
+patinfo_idadmin0,
+patinfo_idadmin1,
+patinfo_idadmin2,
+patinfo_resadmin0,
+patinfo_resadmin1,
+patinfo_resadmin2,
+patcourse_dateonset,
+patcourse_asymp,
+patcourse_dateonset_unk,
+patcourse_admit,
+patcourse_icu,
+patcourse_preshcf,
+patcourse_admitname,
+patcourse_vent,
+patcourse_ecmo,
+patcourse_iso,
+patcourse_dateiso,
+patcourse_status,
+patcourse_datedeath,
+patsympt_fever,
+patsympt_weak,
+patsympt_irritability,
+patsympt_sorethroat,
+patsympt_produ,
+patsympt_runnynose,
+patsympt_short,
+patsympt_diarr,
+patsympt_vomit,
+patsympt_headache,
+patsympt_pain,
+patsympt_muscupain,
+patsympt_chestpain,
+patsympt_abdopain,
+patsympt_jointpain,
+patsympt_other,
+pat_sign_temp,
+pat_sign_temp_unit,
+pat_sign_pharyn,
+pat_sign_conjunc,
+pat_sign_dysp,
+pat_sign_ausc,
+pat_sign_xray,
+pat_sign_seize,
+pat_sign_coma,
+pat_sign_other,
+comcond_present,
+comcond_preg,
+comcond_pregt,
+comcond_partum,
+comcond_immuno,
+comcond_cardi,
+comcond_diabetes,
+comcond_liver,
+comcond_renal,
+comcond_neuro,
+comcond_malig,
+comcond_lung,
+comcond_other,
+(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occus END) AS patinfo_occus,
+patinfo_occuhcw,
+patinfo_occuhcw_country,
+patinfo_occuhcw_city,
+patinfo_occuhcw_name,
+(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occulab END) AS patinfo_occulab,
+(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occuani END) AS patinfo_occuani,
+(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occuother END) AS patinfo_occuother,
+expo_travel,
+(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE expo_travel_country1 END) AS expo_travel_country1,
+expo_travel_city1,
+expo_travel_date1,
+expo_travel_date2,
+expo_travel_date3,
+expo_travel_country2,
+expo_travel_city2,
+expo_travel_country3,
+expo_travel_city3,
+expo_visit_healthcare,
+expo_ari,
+expo_ari_healthcare,
+expo_ari_family,
+expo_ari_workplace,
+expo_ari_settingother,
+expo_ari_settingunknown,
+expo_contact_case,
+expo_case_setting_detail,
+expo_id1,
+expo_case_date_first1,
+expo_case_date_last1,
+expo_id2,
+expo_case_date_first2,
+expo_case_date_last2,
+expo_id3,
+expo_case_date_first3,
+expo_case_date_last3,
+expo_id4,
+expo_case_date_first4,
+expo_case_date_last4,
+expo_id5,
+expo_case_date_first5,
+expo_case_date_last5,
+expo_case_healthcare,
+expo_case_family,
+expo_case_workplace,
+expo_case_settingother,
+expo_case_settingunknown,
+expo_case_location,
+expo_animal,
+expo_animal_location,
+lab_name,
+lab_assay,
+lab_sequencing,
+lab_date1
+FROM who;</t>
+  </si>
+  <si>
+    <t>SELECT pt,
+phacid,
+reporteddate,
+sex,
+sexgender,
+age,
+ageunit,
+onsetdate,
+earliestlabcollectiondate,
+earliestlabtestresultdate,
+phacreporteddate,
+asymptomatic2,
+hospstartdate,
+hospenddate,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
+hospstatus,
+hospitalized,
+intensivecareunit,
+death,
+testingreason,
+testingreasonspec,
+residencecountry,
+detectedatentry,
+dateofentry,
+pointofentrylocation,
+icu,
+icustartdate,
+icuenddate,
+isolation,
+isolationstartdate,
+isolationenddate,
+mechanicalvent,
+ventstartdate,
+ventenddate,
+disposition,
+recoverydate,
+deathcause,
+deathdate,
+coviddeath,
+travel,
+closecontactcase,
+closecontacttravel,
+contactsetting,
+earliestfirstcontactdate,
+healthfacilityexposure,
+numberofcontacts,
+labspecimentype1,
+labtestmethod1,
+labtestresult1,
+(CASE WHEN pt = 'pe' THEN NULL ELSE known_contact END) AS known_contact,
+(CASE WHEN pt = 'pe' THEN NULL ELSE exposurecountry END) AS exposurecountry,
+occupationhcw,
+ltc_resident,
+residency,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupation END) AS occupation,
+(CASE WHEN pt = 'pe' THEN NULL ELSE occupationspec END) AS occupationspec,
+last_refreshed
+FROM modelling_data;</t>
   </si>
 </sst>
 </file>
@@ -299,8 +756,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,7 +1065,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -627,155 +1086,155 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -784,36 +1243,36 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -825,489 +1284,489 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert back to pre sql changes
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="78">
   <si>
     <t>dir</t>
   </si>
@@ -71,12 +71,18 @@
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE</t>
   </si>
   <si>
+    <t>select * from all_cases_web;</t>
+  </si>
+  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/SAS_Analysis/Domestic data</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DASHBOARD</t>
   </si>
   <si>
+    <t>select * from all_cases;</t>
+  </si>
+  <si>
     <t>nm</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
     <t>Dashboard</t>
   </si>
   <si>
+    <t>select * from data_hub;</t>
+  </si>
+  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/Data Requests/SituationalAwareness Dashboard Daily Extract</t>
   </si>
   <si>
@@ -110,6 +119,9 @@
     <t>L:/HPOC/Active Events/001-20 COVID-19/Dashboard</t>
   </si>
   <si>
+    <t>select * from modelling_data;</t>
+  </si>
+  <si>
     <t>STATCAN</t>
   </si>
   <si>
@@ -122,6 +134,9 @@
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/WHO</t>
   </si>
   <si>
+    <t>select * from who;</t>
+  </si>
+  <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
   </si>
   <si>
@@ -224,6 +239,9 @@
     <t>keep_only_web_epi_cols</t>
   </si>
   <si>
+    <t>select * from statscan where classification='confirmed';</t>
+  </si>
+  <si>
     <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
@@ -248,479 +266,7 @@
     <t>trend_extract.xlsx</t>
   </si>
   <si>
-    <t>SELECT phacid,
-pt,
-episodedate,
-classification,
-sex2,
-agegroup10,
-age,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupation2 END) AS occupation2,
-healthcare_worker2,
-ltc_resident2,
-asymptomatic2,
-onsetdate2,
-symcough,
-symfever,
-symchills,
-symsorethroat,
-symrunnynose,
-symshortnessofbreath,
-symnausea,
-symheadache,
-symweakness,
-sympain,
-symirritability,
-symdiarrhea,
-symother,
-symotherspec,
-hospstatus,
-disposition2,
-recoverydate2,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat2 END) AS exposure_cat2
-FROM statscan WHERE  classification='confirmed';</t>
-  </si>
-  <si>
-    <t>SELECT phacid,
-episodedate,
-episodetype,
-sex_excunk,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
-symcough,
-symfever,
-symchills,
-symsorethroat,
-symrunnynose,
-symshortnessofbreath,
-symnausea,
-symheadache,
-symweakness,
-sympain,
-symirritability,
-symdiarrhea,
-symother,
-symotherspec,
-agegroup10,
-agegroup20,
-mechanicalvent,
-hospstatus,
-coviddeath,
-disposition,
-pt,
-last_refreshed
-FROM all_cases_web;</t>
-  </si>
-  <si>
-    <t>SELECT phacid,
-pt,
-ptcaseid,
-phacreporteddate,
-phacreporteddate_epiweek,
-cluster,
-outbreakid,
-outbreak_associated,
-healthregion,
-reporteddate,
-testingreason,
-testingreasonspec,
-classification,
-residency,
-residencecountry,
-detectedatentry,
-dateofentry,
-pointofentrylocation,
-sex,
-gender,
-sexgender,
-age,
-ageunit,
-agegrouping,
-agegroup10,
-agegroup20,
-age_years,
-indigenous,
-(CASE WHEN pt = 'pe' THEN NULL ELSE indigenousidentity END) AS indigenousidentity,
-(CASE WHEN pt = 'pe' THEN NULL ELSE residence_reservecommunitycrownland END) AS residence_reservecommunitycrownland,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupation END) AS occupation,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupationspec END) AS occupationspec,
-occupationhcw,
-occupationhcwrole,
-ltc_resident,
-(CASE WHEN pt = 'pe' THEN NULL ELSE race END) AS race,
-dwellingtype,
-(CASE WHEN pt = 'pe' THEN NULL ELSE fsa END) AS fsa,
-onsetdate,
-onsetdate_epiweek,
-episodedate,
-episodedate_epiweek,
-episodetype,
-earliestdate,
-hosp,
-hospstartdate,
-hospenddate,
-hospstatus,
-hospitalized,
-intensivecareunit,
-icu,
-icustartdate,
-icuenddate,
-isolation,
-isolationstartdate,
-isolationenddate,
-mechanicalvent,
-ventstartdate,
-ventenddate,
-coviddeath,
-disposition,
-recoverydate,
-deathresp,
-deathcause,
-deathdate,
-death,
-travel,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposurecountry END) AS exposurecountry,
-(CASE WHEN pt = 'pe' THEN NULL ELSE location END) AS location,
-travel_domestic,
-travel_international,
-closecontactcase,
-closecontacttravel,
-animalcontact,
-(CASE WHEN pt = 'pe' THEN NULL ELSE known_contact END) AS known_contact,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
-exposure_linked,
-numberofcontacts,
-healthfacilityexposure,
-earliestlabtestresultdate,
-labtestresultdate_epiweek,
-earliestlabcollectiondate,
-labspecimencollectiondate_epiweek,
-minlabname,
-minassay,
-labspecimentype1,
-labtestmethod1,
-labtestresult1,
-rfcardiacdisease,
-rfneurodisorder,
-rfdiabetes,
-rfimmunodef,
-rfliverdisease,
-rfmalignancy,
-rfpostpartum,
-rfpregnancy,
-rfpregtrimester,
-rfrenaldisease,
-rfrespdisease,
-rfvaping,
-rfasthma,
-rfcardiovasculardisease,
-rfcerebrovasculardisease,
-rfchronickidneydisease,
-rfcopd,
-rfhypertension,
-rfobesity,
-rfproblematicsubstanceuse,
-rfsicklecelldisease,
-rfsmokingtobacco,
-rfother,
-rfotherspec,
-rfcount,
-comp_riskfactors,
-asymptomatic2,
-asymptomatic,
-symcount,
-symcough,
-symfever,
-symchills,
-symsorethroat,
-symrunnynose,
-symshortnessofbreath,
-symnausea,
-symheadache,
-symweakness,
-sympain,
-symirritability,
-symdiarrhea,
-symconfusion,
-symchestpain,
-symdizziness,
-symageusia,
-symanosmia,
-symmusclepain,
-symbodyaches,
-symjointpain,
-syminappetence,
-symfatigue,
-symsweats,
-symlocalizedpain,
-symear,
-symnosebleed,
-symeye,
-symcongestion,
-symmalaise,
-symanorexia,
-symskinreactions,
-symsneezing,
-symbreathing,
-symother,
-symotherspec,
-dxlungausc,
-dxlungauscspec,
-dxmentalstatus,
-dxmentalstatusspec,
-dxpneumonia,
-dxpneumoniaspec,
-dxcoma,
-dxcomaspec,
-dxconjunctinjection,
-dxconjunctinjectionspec,
-dxards,
-dxardsspec,
-dxdyspnea,
-dxdyspneaspec,
-dxencephalitis,
-dxencephalitisspec,
-dxhypotension,
-dxhypotensionspec,
-dxpharyngeal,
-dxpharyngealspec,
-dxrenalfailure,
-dxrenalfailurespec,
-dxseizure,
-dxseizurespec,
-dxsepsis,
-dxsepsisspec,
-dxtachypnea,
-dxtachypneaspec,
-dxother,
-dxotherspec,
-contactsetting,
-minsettingspec,
-mincontactcaseid,
-earliestfirstcontactdate,
-latestcontactdate,
-last_refreshed
-FROM all_cases;</t>
-  </si>
-  <si>
-    <t>SELECT episodedate,
-classification,
-pt,
-sexgender2,
-agegroup10,
-age,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupation2 END) AS occupation2,
-occupationhcw,
-ltc_resident,
-asymptomatic2,
-onsetdate2,
-asymptomatic,
-symcough,
-symfever,
-symchills,
-symsorethroat,
-symrunnynose,
-symshortnessofbreath,
-symnausea,
-symheadache,
-symweakness,
-sympain,
-symirritability,
-symdiarrhea,
-symother,
-symotherspec,
-hospstatus,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat2 END) AS exposure_cat2,
-disposition2,
-recoverydate2
-FROM data_hub;</t>
-  </si>
-  <si>
-    <t>SELECT report_date,
-report_orginst,
-report_test_reason,
-report_test_reason_other,
-report_country,
-report_diag_class,
-report_pointofentry,
-report_pointofentry_date,
-patinfo_id,
-patinfo_dob,
-patinfo_ageonset,
-patinfo_ageonsetunit,
-patinfo_sex,
-patinfo_idadmin0,
-patinfo_idadmin1,
-patinfo_idadmin2,
-patinfo_resadmin0,
-patinfo_resadmin1,
-patinfo_resadmin2,
-patcourse_dateonset,
-patcourse_asymp,
-patcourse_dateonset_unk,
-patcourse_admit,
-patcourse_icu,
-patcourse_preshcf,
-patcourse_admitname,
-patcourse_vent,
-patcourse_ecmo,
-patcourse_iso,
-patcourse_dateiso,
-patcourse_status,
-patcourse_datedeath,
-patsympt_fever,
-patsympt_weak,
-patsympt_irritability,
-patsympt_sorethroat,
-patsympt_produ,
-patsympt_runnynose,
-patsympt_short,
-patsympt_diarr,
-patsympt_vomit,
-patsympt_headache,
-patsympt_pain,
-patsympt_muscupain,
-patsympt_chestpain,
-patsympt_abdopain,
-patsympt_jointpain,
-patsympt_other,
-pat_sign_temp,
-pat_sign_temp_unit,
-pat_sign_pharyn,
-pat_sign_conjunc,
-pat_sign_dysp,
-pat_sign_ausc,
-pat_sign_xray,
-pat_sign_seize,
-pat_sign_coma,
-pat_sign_other,
-comcond_present,
-comcond_preg,
-comcond_pregt,
-comcond_partum,
-comcond_immuno,
-comcond_cardi,
-comcond_diabetes,
-comcond_liver,
-comcond_renal,
-comcond_neuro,
-comcond_malig,
-comcond_lung,
-comcond_other,
-(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occus END) AS patinfo_occus,
-patinfo_occuhcw,
-patinfo_occuhcw_country,
-patinfo_occuhcw_city,
-patinfo_occuhcw_name,
-(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occulab END) AS patinfo_occulab,
-(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occuani END) AS patinfo_occuani,
-(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE patinfo_occuother END) AS patinfo_occuother,
-expo_travel,
-(CASE WHEN patinfo_resadmin1 = 'prince edward island' THEN NULL ELSE expo_travel_country1 END) AS expo_travel_country1,
-expo_travel_city1,
-expo_travel_date1,
-expo_travel_date2,
-expo_travel_date3,
-expo_travel_country2,
-expo_travel_city2,
-expo_travel_country3,
-expo_travel_city3,
-expo_visit_healthcare,
-expo_ari,
-expo_ari_healthcare,
-expo_ari_family,
-expo_ari_workplace,
-expo_ari_settingother,
-expo_ari_settingunknown,
-expo_contact_case,
-expo_case_setting_detail,
-expo_id1,
-expo_case_date_first1,
-expo_case_date_last1,
-expo_id2,
-expo_case_date_first2,
-expo_case_date_last2,
-expo_id3,
-expo_case_date_first3,
-expo_case_date_last3,
-expo_id4,
-expo_case_date_first4,
-expo_case_date_last4,
-expo_id5,
-expo_case_date_first5,
-expo_case_date_last5,
-expo_case_healthcare,
-expo_case_family,
-expo_case_workplace,
-expo_case_settingother,
-expo_case_settingunknown,
-expo_case_location,
-expo_animal,
-expo_animal_location,
-lab_name,
-lab_assay,
-lab_sequencing,
-lab_date1
-FROM who;</t>
-  </si>
-  <si>
-    <t>SELECT pt,
-phacid,
-reporteddate,
-sex,
-sexgender,
-age,
-ageunit,
-onsetdate,
-earliestlabcollectiondate,
-earliestlabtestresultdate,
-phacreporteddate,
-asymptomatic2,
-hospstartdate,
-hospenddate,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposure_cat END) AS exposure_cat,
-hospstatus,
-hospitalized,
-intensivecareunit,
-death,
-testingreason,
-testingreasonspec,
-residencecountry,
-detectedatentry,
-dateofentry,
-pointofentrylocation,
-icu,
-icustartdate,
-icuenddate,
-isolation,
-isolationstartdate,
-isolationenddate,
-mechanicalvent,
-ventstartdate,
-ventenddate,
-disposition,
-recoverydate,
-deathcause,
-deathdate,
-coviddeath,
-travel,
-closecontactcase,
-closecontacttravel,
-contactsetting,
-earliestfirstcontactdate,
-healthfacilityexposure,
-numberofcontacts,
-labspecimentype1,
-labtestmethod1,
-labtestresult1,
-(CASE WHEN pt = 'pe' THEN NULL ELSE known_contact END) AS known_contact,
-(CASE WHEN pt = 'pe' THEN NULL ELSE exposurecountry END) AS exposurecountry,
-occupationhcw,
-ltc_resident,
-residency,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupation END) AS occupation,
-(CASE WHEN pt = 'pe' THEN NULL ELSE occupationspec END) AS occupationspec,
-last_refreshed
-FROM modelling_data;</t>
+    <t>{suffix}_HCDaily_DISCOVER_2.xlsx</t>
   </si>
 </sst>
 </file>
@@ -756,10 +302,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1042,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,7 +609,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1086,155 +630,155 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1243,36 +787,36 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -1284,489 +828,489 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="L13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added weekly qry all cases
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="81">
   <si>
     <t>dir</t>
   </si>
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>{suffix}_HCDaily_DISCOVER_2.xlsx</t>
+  </si>
+  <si>
+    <t>epi - weekly</t>
+  </si>
+  <si>
+    <t>keep_only_weekly_report_cols</t>
+  </si>
+  <si>
+    <t>qry_allcases {suffix}_DISCOVER_weekly.xlsx</t>
   </si>
 </sst>
 </file>
@@ -302,8 +311,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,16 +594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:N20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
@@ -702,25 +712,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="L4" t="s">
         <v>61</v>
@@ -728,101 +732,68 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
         <v>61</v>
       </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s">
-        <v>61</v>
-      </c>
       <c r="L6" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -851,19 +822,19 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
         <v>61</v>
@@ -889,19 +860,19 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -930,22 +901,19 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
         <v>61</v>
@@ -971,22 +939,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
       </c>
       <c r="H11" t="s">
         <v>61</v>
@@ -1010,101 +978,128 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s">
+    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
       </c>
       <c r="L13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>77</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" t="s">
+        <v>61</v>
       </c>
       <c r="L14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" t="s">
-        <v>61</v>
-      </c>
-      <c r="M15" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1116,7 +1111,7 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -1154,16 +1149,13 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
         <v>61</v>
@@ -1189,25 +1181,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
         <v>61</v>
@@ -1233,22 +1222,25 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
       </c>
       <c r="H19" t="s">
         <v>61</v>
@@ -1274,48 +1266,89 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
       </c>
       <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="H20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I20" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" t="s">
-        <v>61</v>
-      </c>
-      <c r="K20" t="s">
-        <v>61</v>
-      </c>
-      <c r="L20" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" t="s">
-        <v>61</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" t="s">
+        <v>61</v>
+      </c>
+      <c r="K21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1"/>
+    <hyperlink ref="D18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
date and numeric column formatting adjustment
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="84">
   <si>
     <t>dir</t>
   </si>
@@ -273,6 +273,18 @@
   </si>
   <si>
     <t>DomesticSurveillanceData_{suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>who_cols_formatting</t>
+  </si>
+  <si>
+    <t>dashboard_and_epi_cols_formatting</t>
+  </si>
+  <si>
+    <t>statcan_cols_formatting</t>
+  </si>
+  <si>
+    <t>modelling_cols_formatting</t>
   </si>
 </sst>
 </file>
@@ -593,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,6 +732,9 @@
       <c r="B4" t="s">
         <v>33</v>
       </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
@@ -740,6 +755,9 @@
       <c r="B5" t="s">
         <v>33</v>
       </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
       <c r="D5" t="s">
         <v>34</v>
       </c>
@@ -830,6 +848,9 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -868,6 +889,9 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
@@ -909,6 +933,9 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
@@ -947,6 +974,9 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
@@ -1093,6 +1123,9 @@
       <c r="B15" t="s">
         <v>68</v>
       </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
       <c r="D15" t="s">
         <v>30</v>
       </c>
@@ -1113,6 +1146,9 @@
       <c r="B16" t="s">
         <v>28</v>
       </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
@@ -1151,6 +1187,9 @@
       <c r="B17" t="s">
         <v>28</v>
       </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
       <c r="D17" t="s">
         <v>26</v>
       </c>
@@ -1188,6 +1227,9 @@
       </c>
       <c r="B18" t="s">
         <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
remove rds extracts not required (dashboard, web epi)
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
   <si>
     <t>dir</t>
   </si>
@@ -59,9 +59,6 @@
     <t>remove_pt_cols</t>
   </si>
   <si>
-    <t>qry_allcases_current.rds</t>
-  </si>
-  <si>
     <t>qry_allcases_current.xlsx</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>all_cases_web_current.xlsx</t>
-  </si>
-  <si>
-    <t>all_cases_web_current.rds</t>
   </si>
   <si>
     <t>datahub</t>
@@ -600,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -647,386 +641,377 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
-      </c>
-      <c r="M1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" t="s">
-        <v>60</v>
+      <c r="F9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M12" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1034,320 +1019,256 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="I14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
+        <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" t="s">
-        <v>60</v>
-      </c>
-      <c r="L20" t="s">
-        <v>60</v>
-      </c>
-      <c r="M20" t="s">
-        <v>60</v>
-      </c>
-      <c r="N20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1"/>
+    <hyperlink ref="D15" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
WHO extract col subset
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -266,9 +266,6 @@
     <t>DomesticSurveillanceData_{suffix}_DISCOVER.csv.bz2</t>
   </si>
   <si>
-    <t>who_cols_formatting</t>
-  </si>
-  <si>
     <t>dashboard_and_epi_cols_formatting</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>modelling_cols_formatting</t>
+  </si>
+  <si>
+    <t>keep_only_who_cols</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,7 +696,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -719,7 +719,7 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -812,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -853,7 +853,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -999,7 +999,7 @@
         <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -1022,7 +1022,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -1063,7 +1063,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1104,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
change who to csv and hcdaily to csv.zip
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="82">
   <si>
     <t>dir</t>
   </si>
@@ -140,9 +140,6 @@
     <t>qry_allcases {suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
-    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>Domestic surveillance data - {suffix}_DISCOVER.xlsx</t>
   </si>
   <si>
@@ -276,6 +273,12 @@
   </si>
   <si>
     <t>who_cols_formatting</t>
+  </si>
+  <si>
+    <t>Domestic surveillance data - {suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.csv</t>
   </si>
 </sst>
 </file>
@@ -291,12 +294,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -311,9 +320,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,25 +651,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -670,22 +680,22 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -696,19 +706,19 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -719,89 +729,89 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -812,7 +822,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -824,25 +834,25 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -853,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -865,36 +875,36 @@
         <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -903,10 +913,10 @@
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -923,31 +933,31 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -964,31 +974,31 @@
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -996,22 +1006,22 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1022,7 +1032,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -1031,28 +1041,28 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1063,7 +1073,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1072,28 +1082,28 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1104,166 +1114,166 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>40</v>
       </c>
-      <c r="G16" t="s">
-        <v>41</v>
-      </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change hcdaily to csv
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -275,10 +275,10 @@
     <t>who_cols_formatting</t>
   </si>
   <si>
-    <t>Domestic surveillance data - {suffix}_DISCOVER.csv.bz2</t>
-  </si>
-  <si>
     <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.csv</t>
+  </si>
+  <si>
+    <t>Domestic surveillance data - {suffix}_DISCOVER.csv</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +715,7 @@
         <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>57</v>
@@ -738,7 +738,7 @@
         <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>57</v>
@@ -1041,7 +1041,7 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Change weekly extract days to sunday
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,7 +915,7 @@
       <c r="F9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="H9" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reduce trend epi outputs
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
   <si>
     <t>dir</t>
   </si>
@@ -604,7 +604,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,9 +763,6 @@
       <c r="I5" t="s">
         <v>57</v>
       </c>
-      <c r="L5" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -802,12 +799,6 @@
         <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reduced schedule + #224 adjust weekly extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>dir</t>
   </si>
@@ -300,7 +300,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,7 +615,7 @@
     <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
@@ -688,12 +688,15 @@
       <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
       <c r="M2" t="s">
         <v>57</v>
       </c>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -714,9 +717,15 @@
       <c r="F3" t="s">
         <v>80</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -737,9 +746,15 @@
       <c r="F4" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -760,9 +775,15 @@
       <c r="F5" t="s">
         <v>71</v>
       </c>
+      <c r="H5" s="2"/>
       <c r="I5" t="s">
         <v>57</v>
       </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -801,6 +822,8 @@
       <c r="L6" t="s">
         <v>57</v>
       </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -906,6 +929,12 @@
       <c r="H9" t="s">
         <v>57</v>
       </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1011,6 +1040,12 @@
       <c r="H12" t="s">
         <v>57</v>
       </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1046,12 +1081,8 @@
       <c r="L13" t="s">
         <v>57</v>
       </c>
-      <c r="M13" t="s">
-        <v>57</v>
-      </c>
-      <c r="N13" t="s">
-        <v>57</v>
-      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1116,9 +1147,7 @@
       <c r="G15" t="s">
         <v>69</v>
       </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" t="s">
         <v>57</v>
       </c>
@@ -1134,9 +1163,7 @@
       <c r="M15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
-        <v>57</v>
-      </c>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
#263 WHO extract wednesdays
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,10 +720,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="K3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
@@ -749,10 +749,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="K4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>

</xml_diff>

<commit_message>
#265 change web epi report day
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,10 +692,10 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" t="s">
-        <v>57</v>
-      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
dated web epi extract added
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="83">
   <si>
     <t>dir</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
+  </si>
+  <si>
+    <t>all_cases_web_{suffix}.xlsx</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/All_cases_web_Archive</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,30 +706,30 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" t="s">
+        <v>57</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
@@ -738,7 +744,7 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>49</v>
@@ -758,29 +764,29 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" t="s">
-        <v>57</v>
-      </c>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -802,47 +808,39 @@
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="H6" s="2"/>
       <c r="I6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s">
-        <v>57</v>
-      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
       </c>
       <c r="H7" t="s">
         <v>57</v>
@@ -859,16 +857,12 @@
       <c r="L7" t="s">
         <v>57</v>
       </c>
-      <c r="M7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" t="s">
-        <v>57</v>
-      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -877,105 +871,105 @@
         <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" t="s">
-        <v>57</v>
-      </c>
-      <c r="M8" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
       <c r="H10" t="s">
         <v>57</v>
       </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" t="s">
-        <v>57</v>
-      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -988,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
@@ -1020,67 +1014,71 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
         <v>57</v>
       </c>
-      <c r="I13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" t="s">
-        <v>57</v>
-      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
@@ -1095,7 +1093,7 @@
         <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
@@ -1118,12 +1116,8 @@
       <c r="L14" t="s">
         <v>57</v>
       </c>
-      <c r="M14" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" t="s">
-        <v>57</v>
-      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1136,18 +1130,17 @@
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
       <c r="I15" t="s">
         <v>57</v>
       </c>
@@ -1163,33 +1156,33 @@
       <c r="M15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" t="s">
-        <v>57</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="H16" s="2"/>
       <c r="I16" t="s">
         <v>57</v>
       </c>
@@ -1205,28 +1198,29 @@
       <c r="M16" t="s">
         <v>57</v>
       </c>
-      <c r="N16" t="s">
-        <v>57</v>
-      </c>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
       </c>
       <c r="H17" t="s">
         <v>57</v>
@@ -1252,48 +1246,89 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18" t="s">
-        <v>57</v>
-      </c>
-      <c r="M18" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1"/>
+    <hyperlink ref="D16" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
#199 big_metabase_query adjusted, csv, order by
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -68,18 +68,12 @@
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE</t>
   </si>
   <si>
-    <t>select * from all_cases_web;</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/SAS_Analysis/Domestic data</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DASHBOARD</t>
   </si>
   <si>
-    <t>select * from all_cases;</t>
-  </si>
-  <si>
     <t>nm</t>
   </si>
   <si>
@@ -116,9 +110,6 @@
     <t>L:/HPOC/Active Events/001-20 COVID-19/Dashboard</t>
   </si>
   <si>
-    <t>select * from modelling_data;</t>
-  </si>
-  <si>
     <t>STATCAN</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/WHO</t>
   </si>
   <si>
-    <t>select * from who;</t>
-  </si>
-  <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
   </si>
   <si>
@@ -225,9 +213,6 @@
   </si>
   <si>
     <t>keep_only_web_epi_cols</t>
-  </si>
-  <si>
-    <t>select * from statscan where classification='confirmed';</t>
   </si>
   <si>
     <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
@@ -300,6 +285,21 @@
   </si>
   <si>
     <t>save_csv</t>
+  </si>
+  <si>
+    <t>select * from all_cases_web order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from who order by patinfo_id;</t>
+  </si>
+  <si>
+    <t>select * from statscan where classification='confirmed' order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from modelling_data order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from all_cases order by phacid;</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,8 +328,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -337,15 +343,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +653,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="H2" sqref="H2:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -652,7 +676,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -673,453 +697,453 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>52</v>
-      </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
       <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="H13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -1127,260 +1151,260 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" t="s">
-        <v>57</v>
+      <c r="H14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" t="s">
-        <v>57</v>
-      </c>
-      <c r="N15" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" t="s">
-        <v>57</v>
-      </c>
-      <c r="L17" t="s">
-        <v>57</v>
-      </c>
-      <c r="M17" t="s">
-        <v>57</v>
-      </c>
-      <c r="N17" t="s">
-        <v>57</v>
+        <v>36</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18" t="s">
-        <v>57</v>
-      </c>
-      <c r="M18" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" t="s">
-        <v>57</v>
-      </c>
-      <c r="L19" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" t="s">
-        <v>57</v>
-      </c>
-      <c r="N19" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" t="s">
-        <v>57</v>
-      </c>
-      <c r="L20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M20" t="s">
-        <v>57</v>
-      </c>
-      <c r="N20" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N20" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
#199 order by VOC
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -272,34 +272,34 @@
     <t>voc</t>
   </si>
   <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis</t>
+  </si>
+  <si>
+    <t>all_cases_variants_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>save_csv</t>
+  </si>
+  <si>
+    <t>select * from all_cases_web order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from who order by patinfo_id;</t>
+  </si>
+  <si>
+    <t>select * from statscan where classification='confirmed' order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from modelling_data order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from all_cases order by phacid;</t>
+  </si>
+  <si>
     <t>select  all_cases.*, information_schema.variants.id as variantid, information_schema.variants.identified as variantidentified, information_schema.variants.screenresult as variantscreenresult,information_schema.variants.sequenceresult as variantsequenceresult
         from all_cases
         left join information_schema.variants
-        on all_cases.phacid = information_schema.variants.phacid;</t>
-  </si>
-  <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis</t>
-  </si>
-  <si>
-    <t>all_cases_variants_{suffix}.csv.bz2</t>
-  </si>
-  <si>
-    <t>save_csv</t>
-  </si>
-  <si>
-    <t>select * from all_cases_web order by phacid;</t>
-  </si>
-  <si>
-    <t>select * from who order by patinfo_id;</t>
-  </si>
-  <si>
-    <t>select * from statscan where classification='confirmed' order by phacid;</t>
-  </si>
-  <si>
-    <t>select * from modelling_data order by phacid;</t>
-  </si>
-  <si>
-    <t>select * from all_cases order by phacid;</t>
+        on all_cases.phacid = information_schema.variants.phacid order by phacid;</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:N20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -752,7 +752,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>59</v>
@@ -781,7 +781,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>74</v>
@@ -810,7 +810,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>74</v>
@@ -921,7 +921,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
         <v>72</v>
@@ -950,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>73</v>
@@ -987,7 +987,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>73</v>
@@ -1028,7 +1028,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>73</v>
@@ -1068,7 +1068,7 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>55</v>
@@ -1097,7 +1097,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -1137,7 +1137,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
         <v>71</v>
@@ -1178,7 +1178,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>71</v>
@@ -1219,7 +1219,7 @@
         <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>68</v>
@@ -1248,7 +1248,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
         <v>58</v>
@@ -1292,7 +1292,7 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -1333,7 +1333,7 @@
         <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -1374,19 +1374,19 @@
         <v>78</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
       </c>
       <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
         <v>81</v>
-      </c>
-      <c r="G20" t="s">
-        <v>82</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="5" t="s">

</xml_diff>

<commit_message>
Change all to csv.bz2
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="87">
   <si>
     <t>dir</t>
   </si>
@@ -59,9 +59,6 @@
     <t>remove_pt_cols</t>
   </si>
   <si>
-    <t>qry_allcases_current.xlsx</t>
-  </si>
-  <si>
     <t>saveRDS</t>
   </si>
   <si>
@@ -125,33 +122,18 @@
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
   </si>
   <si>
-    <t>qry_allcases {suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>Domestic surveillance data - {suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>all_cases_web_current.xlsx</t>
-  </si>
-  <si>
     <t>datahub</t>
   </si>
   <si>
     <t>https://storhpocnspdatalakeprod.blob.core.windows.net/hcdaily/data</t>
   </si>
   <si>
-    <t>current_DataHub_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>save_azure</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>CountSummary_{suffix}.xlsx</t>
-  </si>
-  <si>
     <t>countSummary</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
     <t>db_errs</t>
   </si>
   <si>
-    <t>db_errs {suffix}.xlsx</t>
-  </si>
-  <si>
     <t>db_error_report_by_case</t>
   </si>
   <si>
@@ -215,15 +194,9 @@
     <t>keep_only_web_epi_cols</t>
   </si>
   <si>
-    <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/DISCOVER/Data Quality/db_errs</t>
   </si>
   <si>
-    <t>{suffix}_HCDaily_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>https://storphacidpcbns02.blob.core.windows.net/hcdaily</t>
   </si>
   <si>
@@ -233,18 +206,12 @@
     <t>trend_extract.rds</t>
   </si>
   <si>
-    <t>trend_extract.xlsx</t>
-  </si>
-  <si>
     <t>epi - weekly</t>
   </si>
   <si>
     <t>keep_only_weekly_report_cols</t>
   </si>
   <si>
-    <t>qry_allcases {suffix}_DISCOVER_weekly.xlsx</t>
-  </si>
-  <si>
     <t>DomesticSurveillanceData_{suffix}_DISCOVER.csv.bz2</t>
   </si>
   <si>
@@ -260,12 +227,6 @@
     <t>who_cols_formatting</t>
   </si>
   <si>
-    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>all_cases_web_{suffix}.xlsx</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/All_cases_web_Archive</t>
   </si>
   <si>
@@ -276,9 +237,6 @@
   </si>
   <si>
     <t>all_cases_variants_{suffix}.csv.bz2</t>
-  </si>
-  <si>
-    <t>save_csv</t>
   </si>
   <si>
     <t>select * from all_cases_web order by phacid;</t>
@@ -300,6 +258,45 @@
         from all_cases
         left join information_schema.variants
         on all_cases.phacid = information_schema.variants.phacid order by phacid;</t>
+  </si>
+  <si>
+    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>current_DataHub_DISCOVER.xlsx</t>
+  </si>
+  <si>
+    <t>all_cases_web_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>{suffix}_HCDaily_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>Weekly Extended Dataset_{suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>Domestic surveillance data - {suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>trend_extract.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases_current.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases {suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases {suffix}_DISCOVER_weekly.csv.bz2</t>
+  </si>
+  <si>
+    <t>CountSummary_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>db_errs {suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>all_cases_web_current.csv.bz2</t>
   </si>
 </sst>
 </file>
@@ -362,11 +359,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -652,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -676,7 +672,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -697,68 +693,68 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -766,645 +762,642 @@
       <c r="F3" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
         <v>74</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>53</v>
+        <v>77</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>53</v>
+        <v>77</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>53</v>
+        <v>79</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>65</v>
-      </c>
       <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>53</v>
+        <v>81</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>53</v>
+        <v>85</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added trend voc extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
   <si>
     <t>dir</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>save_csv</t>
+  </si>
+  <si>
+    <t>keep_only_trendvoc_epi_cols</t>
+  </si>
+  <si>
+    <t>trendvoc_epi</t>
   </si>
 </sst>
 </file>
@@ -628,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,42 +1047,50 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
+        <v>83</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
+        <v>89</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
@@ -1110,48 +1124,36 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="H14" s="2"/>
       <c r="I14" t="s">
         <v>57</v>
       </c>
-      <c r="J14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" t="s">
-        <v>57</v>
-      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1160,127 +1162,127 @@
         <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
         <v>34</v>
       </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" t="s">
-        <v>57</v>
-      </c>
-      <c r="N15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H16" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" t="s">
-        <v>40</v>
-      </c>
       <c r="H17" t="s">
         <v>57</v>
       </c>
-      <c r="I17" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" t="s">
-        <v>57</v>
-      </c>
-      <c r="L17" t="s">
-        <v>57</v>
-      </c>
-      <c r="M17" t="s">
-        <v>57</v>
-      </c>
-      <c r="N17" t="s">
-        <v>57</v>
-      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -1306,22 +1308,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H19" t="s">
         <v>57</v>
@@ -1347,24 +1349,26 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
       <c r="I20" t="s">
         <v>57</v>
       </c>
@@ -1380,7 +1384,9 @@
       <c r="M20" t="s">
         <v>57</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
extract schedule update, xlsx to csv
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
   <si>
     <t>dir</t>
   </si>
@@ -59,27 +59,18 @@
     <t>remove_pt_cols</t>
   </si>
   <si>
-    <t>qry_allcases_current.xlsx</t>
-  </si>
-  <si>
     <t>saveRDS</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE</t>
   </si>
   <si>
-    <t>select * from all_cases_web;</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/SAS_Analysis/Domestic data</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DASHBOARD</t>
   </si>
   <si>
-    <t>select * from all_cases;</t>
-  </si>
-  <si>
     <t>nm</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>Dashboard</t>
   </si>
   <si>
-    <t>select * from data_hub;</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/Data Requests/SituationalAwareness Dashboard Daily Extract</t>
   </si>
   <si>
@@ -116,9 +104,6 @@
     <t>L:/HPOC/Active Events/001-20 COVID-19/Dashboard</t>
   </si>
   <si>
-    <t>select * from modelling_data;</t>
-  </si>
-  <si>
     <t>STATCAN</t>
   </si>
   <si>
@@ -131,39 +116,21 @@
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/WHO</t>
   </si>
   <si>
-    <t>select * from who;</t>
-  </si>
-  <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
   </si>
   <si>
-    <t>qry_allcases {suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>Domestic surveillance data - {suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>all_cases_web_current.xlsx</t>
-  </si>
-  <si>
     <t>datahub</t>
   </si>
   <si>
     <t>https://storhpocnspdatalakeprod.blob.core.windows.net/hcdaily/data</t>
   </si>
   <si>
-    <t>current_DataHub_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>save_azure</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>CountSummary_{suffix}.xlsx</t>
-  </si>
-  <si>
     <t>countSummary</t>
   </si>
   <si>
@@ -173,9 +140,6 @@
     <t>db_errs</t>
   </si>
   <si>
-    <t>db_errs {suffix}.xlsx</t>
-  </si>
-  <si>
     <t>db_error_report_by_case</t>
   </si>
   <si>
@@ -227,18 +191,9 @@
     <t>keep_only_web_epi_cols</t>
   </si>
   <si>
-    <t>select * from statscan where classification='confirmed';</t>
-  </si>
-  <si>
-    <t>Weekly Extended Dataset_{suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/DISCOVER/Data Quality/db_errs</t>
   </si>
   <si>
-    <t>{suffix}_HCDaily_DISCOVER.xlsx</t>
-  </si>
-  <si>
     <t>https://storphacidpcbns02.blob.core.windows.net/hcdaily</t>
   </si>
   <si>
@@ -248,18 +203,12 @@
     <t>trend_extract.rds</t>
   </si>
   <si>
-    <t>trend_extract.xlsx</t>
-  </si>
-  <si>
     <t>epi - weekly</t>
   </si>
   <si>
     <t>keep_only_weekly_report_cols</t>
   </si>
   <si>
-    <t>qry_allcases {suffix}_DISCOVER_weekly.xlsx</t>
-  </si>
-  <si>
     <t>DomesticSurveillanceData_{suffix}_DISCOVER.csv.bz2</t>
   </si>
   <si>
@@ -275,37 +224,82 @@
     <t>who_cols_formatting</t>
   </si>
   <si>
-    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.xlsx</t>
-  </si>
-  <si>
-    <t>all_cases_web_{suffix}.xlsx</t>
-  </si>
-  <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/All_cases_web_Archive</t>
   </si>
   <si>
     <t>voc</t>
+  </si>
+  <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis</t>
+  </si>
+  <si>
+    <t>all_cases_variants_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>keep_only_trendvoc_epi_cols</t>
+  </si>
+  <si>
+    <t>trendvoc_epi</t>
+  </si>
+  <si>
+    <t>select * from all_cases_web order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from who order by patinfo_id;</t>
+  </si>
+  <si>
+    <t>select * from statscan where classification='confirmed' order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from modelling_data order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from all_cases order by phacid;</t>
   </si>
   <si>
     <t>select  all_cases.*, information_schema.variants.id as variantid, information_schema.variants.identified as variantidentified, information_schema.variants.screenresult as variantscreenresult,information_schema.variants.sequenceresult as variantsequenceresult
         from all_cases
         left join information_schema.variants
-        on all_cases.phacid = information_schema.variants.phacid;</t>
-  </si>
-  <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis</t>
-  </si>
-  <si>
-    <t>all_cases_variants_{suffix}.csv.bz2</t>
-  </si>
-  <si>
-    <t>save_csv</t>
-  </si>
-  <si>
-    <t>keep_only_trendvoc_epi_cols</t>
-  </si>
-  <si>
-    <t>trendvoc_epi</t>
+        on all_cases.phacid = information_schema.variants.phacid order by phacid;</t>
+  </si>
+  <si>
+    <t>select * from data_hub order by phacid;</t>
+  </si>
+  <si>
+    <t>all_cases_web_current.csv.bz2</t>
+  </si>
+  <si>
+    <t>all_cases_web_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>Canada_COVID19_WHO_linelist-{suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>{suffix}_HCDaily_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>Weekly Extended Dataset_{suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>trend_extract.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases_current.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases {suffix}_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>qry_allcases {suffix}_DISCOVER_weekly.csv.bz2</t>
+  </si>
+  <si>
+    <t>current_DataHub_DISCOVER.csv.bz2</t>
+  </si>
+  <si>
+    <t>CountSummary_{suffix}.csv.bz2</t>
+  </si>
+  <si>
+    <t>db_errs_{suffix}.csv.bz2</t>
   </si>
 </sst>
 </file>
@@ -321,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,13 +635,13 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.90625" customWidth="1"/>
     <col min="3" max="3" width="26.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="217.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
@@ -658,7 +658,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -679,109 +679,109 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
         <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -789,28 +789,28 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -818,107 +818,107 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -929,221 +929,208 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" t="s">
-        <v>57</v>
-      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1153,107 +1140,107 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1264,128 +1251,128 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="L20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="M20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="N20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VOC extract query update
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -299,6 +299,9 @@
     <t>db_errs_{suffix}.csv.bz2</t>
   </si>
   <si>
+    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis/Data</t>
+  </si>
+  <si>
     <t>select 
 t1.phacid,
 earliestdate,
@@ -333,10 +336,7 @@
 travel_international,
 exposurecountry
 from all_cases t1 
-left outer join information_schema.variants t2 on t1.phacid=t2.phacid</t>
-  </si>
-  <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis/Data</t>
+left outer join information_schema.variants t2 on t1.phacid=t2.phacid order by phacid;</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1088,10 +1088,10 @@
         <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
         <v>87</v>
-      </c>
-      <c r="D12" t="s">
-        <v>88</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
remove and update adjust functions
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t>dir</t>
   </si>
@@ -210,18 +210,6 @@
   </si>
   <si>
     <t>DomesticSurveillanceData_{suffix}_DISCOVER.csv.bz2</t>
-  </si>
-  <si>
-    <t>dashboard_and_epi_cols_formatting</t>
-  </si>
-  <si>
-    <t>statcan_cols_formatting</t>
-  </si>
-  <si>
-    <t>modelling_cols_formatting</t>
-  </si>
-  <si>
-    <t>who_cols_formatting</t>
   </si>
   <si>
     <t>//Ncr-a_irbv2s/irbv2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/All_cases_web_Archive</t>
@@ -352,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +350,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,11 +366,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -672,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -743,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -755,7 +736,7 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -772,19 +753,19 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -801,10 +782,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -813,7 +791,7 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -830,10 +808,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -842,7 +817,7 @@
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -859,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -871,7 +846,7 @@
         <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H6" t="s">
         <v>45</v>
@@ -900,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -912,7 +887,7 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s">
         <v>45</v>
@@ -941,10 +916,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -953,7 +925,7 @@
         <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
         <v>45</v>
@@ -970,10 +942,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1007,10 +976,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1048,10 +1014,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>53</v>
@@ -1085,47 +1048,47 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>88</v>
+        <v>60</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="I12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -1162,7 +1125,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
@@ -1174,7 +1137,7 @@
         <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="s">
@@ -1191,10 +1154,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1203,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H15" t="s">
         <v>45</v>
@@ -1232,10 +1192,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1244,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
@@ -1273,7 +1230,7 @@
         <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>57</v>
@@ -1285,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
         <v>45</v>
@@ -1302,7 +1259,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
@@ -1314,7 +1271,7 @@
         <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
         <v>30</v>
@@ -1346,7 +1303,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -1358,7 +1315,7 @@
         <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
         <v>45</v>
@@ -1387,7 +1344,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
@@ -1399,7 +1356,7 @@
         <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
updated datahub extract query
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -654,7 +654,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,61 +913,71 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>80</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
       </c>
       <c r="H8" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="I9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" t="s">
-        <v>45</v>
-      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
@@ -979,7 +989,7 @@
         <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1002,12 +1012,8 @@
       <c r="L10" t="s">
         <v>45</v>
       </c>
-      <c r="M10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" t="s">
-        <v>45</v>
-      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1017,7 +1023,7 @@
         <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
@@ -1025,10 +1031,9 @@
       <c r="F11" t="s">
         <v>58</v>
       </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="2"/>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" t="s">
         <v>45</v>
       </c>
@@ -1044,91 +1049,90 @@
       <c r="M11" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" t="s">
         <v>45</v>
       </c>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -1137,71 +1141,73 @@
         <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
       <c r="I14" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" t="s">
+        <v>45</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" t="s">
-        <v>45</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="H15" s="2"/>
       <c r="I15" t="s">
         <v>45</v>
       </c>
-      <c r="J15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" t="s">
-        <v>45</v>
-      </c>
-      <c r="M15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
@@ -1225,78 +1231,72 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>56</v>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>79</v>
+      <c r="F17" t="s">
+        <v>78</v>
       </c>
       <c r="H17" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>28</v>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="H18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" t="s">
-        <v>45</v>
-      </c>
-      <c r="L18" t="s">
-        <v>45</v>
-      </c>
-      <c r="M18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N18" t="s">
-        <v>45</v>
-      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1382,7 +1382,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
adjust qry all cases (drop mincontactcaseid) and add trend epi variables
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
   <si>
     <t>dir</t>
   </si>
@@ -249,18 +249,6 @@
   </si>
   <si>
     <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/PUBLIC HEALTH PROTECTION AND PROMOTION HC8/SURVEILLANCE/COVID/PLANNING/12 - VOC/Analysis/Data</t>
-  </si>
-  <si>
-    <t>select 
-t1.phacid, phacreporteddate, episodedate, pt, age_years, agegroup10, agegroup20, onsetdate, earliestlabcollectiondate, sex, gender, sexgender, coviddeath, hosp, icu, exposure_cat, earliestdate, earliestdatetype, 
-identified,
-screenresult,
-screen_interpreted,
-sequenceresult,
-sequence_interpreted,
-voc_interpreted
-from all_cases t1 
-left outer join information_schema.variants t2 on t1.phacid=t2.phacid order by phacid;</t>
   </si>
   <si>
     <t>select 
@@ -301,6 +289,21 @@
 exposurecountry
 from all_cases t1 
 left outer join information_schema.variants t2 on t1.phacid=t2.phacid order by phacid;</t>
+  </si>
+  <si>
+    <t>select 
+t1.phacid, phacreporteddate, episodedate, pt, age, ageunit, age_years, agegroup10, agegroup20, onsetdate, earliestlabcollectiondate, sex, gender, sexgender, coviddeath, hosp, hospstatus, hospitalized, icu, exposure_cat,  travel, exposure_linked, closecontactcase, closecontacttravel, outbreak_associated, earliestdate, earliestdatetype, 
+identified,
+screenresult,
+screen_interpreted,
+sequenceresult,
+sequence_interpreted,
+voc_interpreted
+from all_cases t1 
+left outer join information_schema.variants t2 on t1.phacid=t2.phacid order by phacid;</t>
+  </si>
+  <si>
+    <t>remove_retired_cols</t>
   </si>
 </sst>
 </file>
@@ -629,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,7 +703,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
@@ -1050,7 +1053,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
@@ -1114,6 +1117,9 @@
       </c>
       <c r="B14" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
remove duplicate WHO extract
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
   <si>
     <t>dir</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>WHO</t>
-  </si>
-  <si>
-    <t>//Ncr-a_irbv2s/IRBV2/PHAC/IDPCB/CIRID/VIPS-SAR/EMERGENCY PREPAREDNESS AND RESPONSE HC4/EMERGENCY EVENT/WUHAN UNKNOWN PNEU - 2020/DATA AND ANALYSIS/DATABASE/OUTPUTS/WHO</t>
   </si>
   <si>
     <t>L:/HPOC/Active Events/001-20 COVID-19/Operations/Surveillance - Epi. Diagnostics/Canada_COVID19_WHO_linelist</t>
@@ -630,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,60 +674,60 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -740,22 +737,22 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -763,179 +760,187 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
@@ -944,255 +949,262 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2"/>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" t="s">
-        <v>41</v>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
       <c r="I13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L14" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" t="s">
-        <v>41</v>
-      </c>
-      <c r="N14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
@@ -1201,71 +1213,30 @@
         <v>69</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" t="s">
-        <v>41</v>
-      </c>
-      <c r="N17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
changed order of trend extracts
</commit_message>
<xml_diff>
--- a/metabase_extracts.xlsx
+++ b/metabase_extracts.xlsx
@@ -630,7 +630,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,70 +734,63 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -810,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -842,25 +835,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
         <v>40</v>
@@ -886,61 +876,71 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>40</v>
-      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
@@ -952,7 +952,7 @@
         <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -975,12 +975,8 @@
       <c r="L9" t="s">
         <v>40</v>
       </c>
-      <c r="M9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" t="s">
-        <v>40</v>
-      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -990,7 +986,7 @@
         <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -998,10 +994,9 @@
       <c r="F10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="2"/>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
       <c r="I10" t="s">
         <v>40</v>
       </c>
@@ -1017,38 +1012,43 @@
       <c r="M10" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" t="s">
         <v>40</v>
       </c>
       <c r="N11" s="2"/>
@@ -1236,7 +1236,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>